<commit_message>
add fft diagram from excel
</commit_message>
<xml_diff>
--- a/Lab 2/FFT/IR_6.08kHz_18kHz_with lowpass filter.xlsx
+++ b/Lab 2/FFT/IR_6.08kHz_18kHz_with lowpass filter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Cornell\Fall 2018\ECE 3400 Physical Intelligent Systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\github\ece-3400-group.github.io\Lab 2\FFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15367,6 +15367,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>IR FFT Diagram</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -18458,38 +18483,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-TW"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -21457,10 +21450,10 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>